<commit_message>
Actualización del Product Backlog con Sprint 1 finalizado
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnovo\Documents\Ingenieria Informatica\2º\Proyecto de Informática 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1597179E7786AF4B/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A247FA7-D42E-4EF0-8085-857CDD7CC62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81551010-391D-4987-9737-5DCE46EE9019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4608" yWindow="1452" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Seguimiento de un proyecto" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -102,10 +102,16 @@
     <t>PRIMER SPRINT</t>
   </si>
   <si>
-    <t>Sin empezar</t>
+    <t>11.30</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
   <si>
     <t>Importante</t>
+  </si>
+  <si>
+    <t>David Novo, Gabriel Rodríguez, Brent Delgado, Lucía Sánchez</t>
   </si>
   <si>
     <r>
@@ -153,6 +159,12 @@
     </r>
   </si>
   <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Brent Delgado, Lucía Sánchez</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -183,6 +195,9 @@
     <t>Diseño de un login para Trabajador y Administrador con acceso de Id y contraseña.</t>
   </si>
   <si>
+    <t>David Novo, Gabriel Rodríguez</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -216,6 +231,9 @@
     <t>SEGUNDO SPRINT</t>
   </si>
   <si>
+    <t>Sin empezar</t>
+  </si>
+  <si>
     <t>Como administrador quiero poder añadir usuarios (trabajadores o administradores)</t>
   </si>
   <si>
@@ -318,7 +336,7 @@
     <numFmt numFmtId="165" formatCode="0\ %"/>
     <numFmt numFmtId="166" formatCode="dd&quot;/&quot;mm&quot;/&quot;yy"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -693,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -882,8 +900,8 @@
     <xf numFmtId="0" fontId="29" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="28" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -896,9 +914,6 @@
     <xf numFmtId="166" fontId="20" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -908,18 +923,38 @@
     <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="29" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -932,20 +967,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,9 +1040,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1059,7 +1080,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1165,7 +1186,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1307,7 +1328,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,41 +1342,41 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="5" width="15.109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="5" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="41.44140625" customWidth="1"/>
-    <col min="9" max="9" width="35.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
-    <col min="11" max="12" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="41.42578125" customWidth="1"/>
+    <col min="9" max="9" width="35.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="58.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-    </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="87"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+    </row>
+    <row r="2" spans="1:13" ht="21" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1369,43 +1390,43 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="34.5" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="82" t="s">
+      <c r="C3" s="86"/>
+      <c r="D3" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
       <c r="H3" s="27"/>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
       <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="40.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="77"/>
+      <c r="C4" s="86"/>
       <c r="D4" s="35"/>
       <c r="E4" s="58"/>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="85"/>
+      <c r="G4" s="94"/>
       <c r="H4" s="28"/>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="73" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="34">
@@ -1415,7 +1436,7 @@
       <c r="L4" s="32"/>
       <c r="M4" s="33"/>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="21" customHeight="1">
       <c r="A5" s="11"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
@@ -1429,7 +1450,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="21" customHeight="1">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1443,27 +1464,27 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="21" customHeight="1">
       <c r="A7" s="15"/>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="75" t="s">
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="90" t="s">
+      <c r="K7" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="91"/>
-    </row>
-    <row r="8" spans="1:13" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="82"/>
+    </row>
+    <row r="8" spans="1:13" ht="35.450000000000003" customHeight="1">
       <c r="A8" s="16"/>
       <c r="B8" s="39" t="s">
         <v>11</v>
@@ -1495,7 +1516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" ht="23.25" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="66" t="s">
         <v>20</v>
@@ -1508,117 +1529,123 @@
       <c r="H9" s="67"/>
       <c r="I9" s="67"/>
       <c r="J9" s="68">
-        <v>0</v>
+        <v>0.9667</v>
       </c>
       <c r="K9" s="69">
-        <v>12</v>
-      </c>
-      <c r="L9" s="70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="L9" s="70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="55.5" customHeight="1">
       <c r="A10" s="17"/>
       <c r="B10" s="59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="61"/>
       <c r="E10" s="61"/>
       <c r="F10" s="60">
         <v>1</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="73" t="s">
+      <c r="G10" s="76" t="s">
         <v>24</v>
       </c>
+      <c r="H10" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>26</v>
+      </c>
       <c r="J10" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="60">
         <v>1</v>
       </c>
       <c r="L10" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="66" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="59" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C11" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
       <c r="F11" s="62">
         <v>1</v>
       </c>
-      <c r="G11" s="72"/>
-      <c r="H11" s="73" t="s">
-        <v>25</v>
+      <c r="G11" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="72" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J11" s="64">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K11" s="60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="53.25" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="61"/>
       <c r="E12" s="61"/>
       <c r="F12" s="62">
         <v>1</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="73" t="s">
-        <v>27</v>
+      <c r="G12" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="72" t="s">
+        <v>32</v>
       </c>
       <c r="I12" s="60" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="J12" s="64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="60">
-        <v>8</v>
-      </c>
-      <c r="L12" s="65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="L12" s="75">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="23.25" customHeight="1">
       <c r="A13" s="17"/>
-      <c r="B13" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
+      <c r="B13" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
       <c r="J13" s="51">
         <v>0</v>
       </c>
@@ -1629,13 +1656,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="83.25" customHeight="1">
       <c r="A14" s="56"/>
       <c r="B14" s="59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="61"/>
       <c r="E14" s="61"/>
@@ -1644,10 +1671,10 @@
       </c>
       <c r="G14" s="63"/>
       <c r="H14" s="60" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I14" s="60" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J14" s="64">
         <v>0</v>
@@ -1659,13 +1686,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="83.25" customHeight="1">
       <c r="A15" s="56"/>
       <c r="B15" s="59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C15" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" s="61"/>
       <c r="E15" s="61"/>
@@ -1674,10 +1701,10 @@
       </c>
       <c r="G15" s="63"/>
       <c r="H15" s="60" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I15" s="60" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="J15" s="64">
         <v>0</v>
@@ -1689,13 +1716,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="83.25" customHeight="1">
       <c r="A16" s="56"/>
       <c r="B16" s="59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C16" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" s="61"/>
       <c r="E16" s="61"/>
@@ -1704,10 +1731,10 @@
       </c>
       <c r="G16" s="63"/>
       <c r="H16" s="60" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J16" s="64">
         <v>0</v>
@@ -1719,13 +1746,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="83.25" customHeight="1">
       <c r="A17" s="56"/>
       <c r="B17" s="59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="61"/>
       <c r="E17" s="61"/>
@@ -1734,10 +1761,10 @@
       </c>
       <c r="G17" s="63"/>
       <c r="H17" s="60" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="I17" s="60" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="J17" s="64">
         <v>0</v>
@@ -1749,13 +1776,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="83.25" customHeight="1">
       <c r="A18" s="56"/>
       <c r="B18" s="59" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C18" s="60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D18" s="61"/>
       <c r="E18" s="61"/>
@@ -1764,10 +1791,10 @@
       </c>
       <c r="G18" s="63"/>
       <c r="H18" s="60" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I18" s="60" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="J18" s="64">
         <v>0</v>
@@ -1779,18 +1806,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" ht="24.75" customHeight="1">
       <c r="A19" s="56"/>
-      <c r="B19" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="89"/>
-      <c r="H19" s="89"/>
-      <c r="I19" s="89"/>
+      <c r="B19" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="51">
         <v>0</v>
       </c>
@@ -1801,13 +1828,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="61.5" customHeight="1">
       <c r="A20" s="23"/>
       <c r="B20" s="43" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="36"/>
       <c r="E20" s="36"/>
@@ -1816,10 +1843,10 @@
       </c>
       <c r="G20" s="44"/>
       <c r="H20" s="44" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I20" s="44" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J20" s="49">
         <v>0</v>
@@ -1831,13 +1858,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="61.5" customHeight="1">
       <c r="A21" s="23"/>
       <c r="B21" s="43" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -1846,10 +1873,10 @@
       </c>
       <c r="G21" s="44"/>
       <c r="H21" s="44" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I21" s="44" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J21" s="49">
         <v>0</v>
@@ -1861,13 +1888,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="96" customHeight="1">
       <c r="A22" s="23"/>
       <c r="B22" s="43" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" s="36"/>
       <c r="E22" s="36"/>
@@ -1876,10 +1903,10 @@
       </c>
       <c r="G22" s="44"/>
       <c r="H22" s="44" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I22" s="44" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J22" s="49">
         <v>0</v>
@@ -1891,13 +1918,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="83.25" customHeight="1">
       <c r="A23" s="23"/>
       <c r="B23" s="43" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="36"/>
@@ -1906,10 +1933,10 @@
       </c>
       <c r="G23" s="44"/>
       <c r="H23" s="44" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I23" s="44" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J23" s="49">
         <v>0</v>
@@ -1921,18 +1948,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" ht="24.75" customHeight="1">
       <c r="A24" s="17"/>
-      <c r="B24" s="86" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="B24" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="78"/>
+      <c r="H24" s="78"/>
+      <c r="I24" s="78"/>
       <c r="J24" s="51">
         <v>0</v>
       </c>
@@ -1943,13 +1970,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="62.25" customHeight="1">
       <c r="A25" s="56"/>
       <c r="B25" s="46" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C25" s="47" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -1958,10 +1985,10 @@
       </c>
       <c r="G25" s="38"/>
       <c r="H25" s="47" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I25" s="47" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J25" s="53">
         <v>0</v>
@@ -1973,13 +2000,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="73.5" customHeight="1">
       <c r="A26" s="56"/>
       <c r="B26" s="46" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
@@ -1988,10 +2015,10 @@
       </c>
       <c r="G26" s="38"/>
       <c r="H26" s="47" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="I26" s="47" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="J26" s="53">
         <v>0</v>
@@ -2003,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="18" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -2017,13 +2044,13 @@
       <c r="K27" s="21"/>
       <c r="L27" s="18"/>
     </row>
-    <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="30" customHeight="1">
       <c r="A28" s="56"/>
       <c r="B28" s="22" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D28" s="57"/>
       <c r="E28" s="57"/>
@@ -2035,13 +2062,13 @@
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
     </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1">
       <c r="A29" s="56"/>
       <c r="B29" s="25" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D29" s="57"/>
       <c r="E29" s="57"/>
@@ -2053,13 +2080,13 @@
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
     </row>
-    <row r="30" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="19.5" customHeight="1">
       <c r="A30" s="56"/>
       <c r="B30" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="57"/>
@@ -2071,13 +2098,13 @@
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
     </row>
-    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1">
       <c r="A31" s="56"/>
       <c r="B31" s="25" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D31" s="57"/>
       <c r="E31" s="57"/>
@@ -2089,11 +2116,11 @@
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
     </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="18" customHeight="1">
       <c r="A32" s="56"/>
       <c r="B32" s="19"/>
       <c r="C32" s="25" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D32" s="57"/>
       <c r="E32" s="57"/>
@@ -2105,7 +2132,7 @@
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
     </row>
-    <row r="33" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="18" customHeight="1">
       <c r="A33" s="56"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -2119,7 +2146,7 @@
       <c r="K33" s="21"/>
       <c r="L33" s="18"/>
     </row>
-    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="18" customHeight="1">
       <c r="A34" s="56"/>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
@@ -2135,11 +2162,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B7:I7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="J1:L1"/>
@@ -2147,6 +2169,11 @@
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="B7:I7"/>
   </mergeCells>
   <conditionalFormatting sqref="K8">
     <cfRule type="colorScale" priority="1">

</xml_diff>